<commit_message>
tranverse gamma in pie dataset
</commit_message>
<xml_diff>
--- a/results/mk-mmcd.xlsx
+++ b/results/mk-mmcd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caokang/Documents/MEDA/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92452EB-1AB1-EE45-902A-8EFF4A01591A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DC644E-92FA-A745-8FE9-81FB15046ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16240" xr2:uid="{21FD61EE-2419-D345-9765-2E447AB1C80B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{21FD61EE-2419-D345-9765-2E447AB1C80B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>MEDA</t>
   </si>
@@ -555,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DD1D7E-C6DB-B14F-BED2-9726A1A9321D}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:I26" si="0">C2-$B2</f>
+        <f t="shared" ref="C15:H26" si="0">C2-$B2</f>
         <v>1.0438413361170129E-3</v>
       </c>
       <c r="D15" s="1">
@@ -957,7 +957,7 @@
         <v>4.4067796610169019E-2</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" ref="H16:I16" si="1">H3-$B3</f>
+        <f t="shared" ref="H16" si="1">H3-$B3</f>
         <v>3.3898305084739677E-3</v>
       </c>
     </row>
@@ -986,7 +986,7 @@
         <v>8.2802547770701063E-2</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17:I17" si="2">H4-$B4</f>
+        <f t="shared" ref="H17" si="2">H4-$B4</f>
         <v>0</v>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" ref="H18:I18" si="3">H5-$B5</f>
+        <f t="shared" ref="H18" si="3">H5-$B5</f>
         <v>6.2333036509349959E-3</v>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
         <v>-6.1016949152542965E-2</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:I19" si="4">H6-$B6</f>
+        <f t="shared" ref="H19" si="4">H6-$B6</f>
         <v>1.6949152542372059E-2</v>
       </c>
     </row>
@@ -1073,7 +1073,7 @@
         <v>-6.3694267515930214E-3</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" ref="H20:I20" si="5">H7-$B7</f>
+        <f t="shared" ref="H20" si="5">H7-$B7</f>
         <v>0</v>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
         <v>1.157613535173696E-2</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" ref="H21:I21" si="6">H8-$B8</f>
+        <f t="shared" ref="H21" si="6">H8-$B8</f>
         <v>-4.4523597506680446E-3</v>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
         <v>-7.3068893528179801E-3</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" ref="H22:I22" si="7">H9-$B9</f>
+        <f t="shared" ref="H22" si="7">H9-$B9</f>
         <v>2.0876826722340258E-3</v>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
         <v>-0.10191082802547802</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" ref="H23:I23" si="8">H10-$B10</f>
+        <f t="shared" ref="H23" si="8">H10-$B10</f>
         <v>0</v>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
         <v>1.6918967052537981E-2</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" ref="H24:I24" si="9">H11-$B11</f>
+        <f t="shared" ref="H24" si="9">H11-$B11</f>
         <v>1.7809439002670069E-3</v>
       </c>
     </row>
@@ -1218,7 +1218,7 @@
         <v>-4.1753653444679961E-3</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" ref="H25:I25" si="10">H12-$B12</f>
+        <f t="shared" ref="H25" si="10">H12-$B12</f>
         <v>3.131524008349984E-3</v>
       </c>
     </row>
@@ -1247,13 +1247,13 @@
         <v>-4.7457627118643986E-2</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" ref="H26:I26" si="11">H13-$B13</f>
+        <f t="shared" ref="H26" si="11">H13-$B13</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
-        <f t="shared" ref="C28:I28" si="12">SUM(C15:C26)/12</f>
+        <f t="shared" ref="C28:H28" si="12">SUM(C15:C26)/12</f>
         <v>8.8006433334015723E-3</v>
       </c>
       <c r="D28" s="1">
@@ -1433,7 +1433,7 @@
         <v>4.0677966101695051E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1443,7 +1443,7 @@
         <v>3.1847133757960999E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
         <f t="shared" si="14"/>
         <v>-1.7809439002670069E-3</v>
@@ -1453,7 +1453,7 @@
         <v>2.6714158504009822E-3</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1463,7 +1463,7 @@
         <v>3.1315240083510387E-3</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" s="1">
         <f t="shared" si="14"/>
         <v>6.3694267515919112E-3</v>
@@ -1473,7 +1473,7 @@
         <v>-2.5477707006368977E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" s="1">
         <f t="shared" si="14"/>
         <v>8.9047195013397529E-4</v>
@@ -1483,7 +1483,7 @@
         <v>8.0142475512020028E-3</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
         <f t="shared" si="14"/>
         <v>5.2192066805839543E-3</v>
@@ -1493,7 +1493,7 @@
         <v>1.0438413361170129E-3</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
         <f t="shared" si="14"/>
         <v>0</v>
@@ -1503,15 +1503,18 @@
         <v>-1.3559322033898979E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C57" s="1">
         <f>SUM(C44:C55)/12</f>
         <v>1.4350769905895183E-2</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B59" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>3</v>
@@ -1519,8 +1522,11 @@
       <c r="D59" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60" s="1">
         <v>0.89</v>
       </c>
@@ -1530,8 +1536,11 @@
       <c r="D60" s="1">
         <v>0.72222222222222199</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="1">
+        <v>0.90222222222222204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" s="1">
         <v>0.748</v>
       </c>
@@ -1541,31 +1550,42 @@
       <c r="D61" s="1">
         <v>0.62549999999999994</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="1">
+        <v>0.73799999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C64" s="1">
-        <f>C60-$B60</f>
+        <f t="shared" ref="C64:E65" si="15">C60-$B60</f>
         <v>-2.77777777777799E-3</v>
       </c>
       <c r="D64" s="1">
-        <f>D60-$B60</f>
+        <f t="shared" si="15"/>
         <v>-0.16777777777777803</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="1">
+        <f t="shared" si="15"/>
+        <v>1.2222222222222023E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C65" s="1">
-        <f>C61-$B61</f>
+        <f t="shared" si="15"/>
         <v>-1.2499999999999956E-2</v>
       </c>
       <c r="D65" s="1">
-        <f>D61-$B61</f>
+        <f t="shared" si="15"/>
         <v>-0.12250000000000005</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65" s="1">
+        <f t="shared" si="15"/>
+        <v>-1.0000000000000009E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
         <v>20</v>
       </c>
@@ -1573,8 +1593,16 @@
         <f>AVERAGE(C64:C65)</f>
         <v>-7.6388888888889728E-3</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="1">
+        <f>AVERAGE(D64:D65)</f>
+        <v>-0.14513888888888904</v>
+      </c>
+      <c r="E67" s="1">
+        <f>AVERAGE(E64:E65)</f>
+        <v>1.1111111111110072E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>22</v>
       </c>
@@ -1582,84 +1610,154 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B71" s="1">
         <v>0.39472068753836698</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="1">
+        <v>0.39410681399631697</v>
+      </c>
+      <c r="D71" s="1">
+        <f>C71-B71</f>
+        <v>-6.13873542050003E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B72" s="1">
         <v>0.44607843137254899</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C72" s="1">
+        <v>0.45955882352941202</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" ref="D72:D90" si="16">C72-B72</f>
+        <v>1.348039215686303E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="1">
         <v>0.64854310603784904</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="1">
+        <v>0.63172123760889198</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.6821868428957054E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B74" s="1">
         <v>0.340073529411765</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="1">
+        <v>0.33762254901960798</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="16"/>
+        <v>-2.4509803921570206E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B75" s="1">
         <v>0.46278511404561801</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="1">
+        <v>0.44327731092437</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.9507803121248002E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B76" s="1">
         <v>0.50796568627451</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C76" s="1">
+        <v>0.50919117647058798</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="16"/>
+        <v>1.2254901960779829E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B77" s="1">
         <v>0.71312706518474001</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C77" s="1">
+        <v>0.690297386602583</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="16"/>
+        <v>-2.2829678582157009E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B78" s="1">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="1">
+        <v>0.36151960784313703</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.3480392156862975E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B79" s="1">
         <v>0.46878751500600202</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="1">
+        <v>0.45378151260504201</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.5006002400960006E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B80" s="1">
         <v>0.488029465930018</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0.46531614487415601</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="16"/>
+        <v>-2.271332105586199E-2</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -1669,6 +1767,13 @@
       <c r="B81" s="1">
         <v>0.72874737158305802</v>
       </c>
+      <c r="C81" s="1">
+        <v>0.71312706518474001</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.5620306398318018E-2</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
@@ -1677,6 +1782,13 @@
       <c r="B82" s="1">
         <v>0.45465686274509798</v>
       </c>
+      <c r="C82" s="1">
+        <v>0.43443627450980399</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="16"/>
+        <v>-2.022058823529399E-2</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
@@ -1685,6 +1797,13 @@
       <c r="B83" s="1">
         <v>0.70048019207683099</v>
       </c>
+      <c r="C83" s="1">
+        <v>0.69477791116446597</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="16"/>
+        <v>-5.7022809123650209E-3</v>
+      </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
@@ -1693,6 +1812,13 @@
       <c r="B84" s="1">
         <v>0.74708410067526099</v>
       </c>
+      <c r="C84" s="1">
+        <v>0.71332105586249195</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="16"/>
+        <v>-3.3763044812769039E-2</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
@@ -1701,6 +1827,13 @@
       <c r="B85" s="1">
         <v>0.82046568627451</v>
       </c>
+      <c r="C85" s="1">
+        <v>0.77450980392156898</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="16"/>
+        <v>-4.5955882352941013E-2</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
@@ -1709,6 +1842,13 @@
       <c r="B86" s="1">
         <v>0.54901960784313697</v>
       </c>
+      <c r="C86" s="1">
+        <v>0.52389705882352899</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="16"/>
+        <v>-2.5122549019607976E-2</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
@@ -1717,6 +1857,13 @@
       <c r="B87" s="1">
         <v>0.38955582232893199</v>
       </c>
+      <c r="C87" s="1">
+        <v>0.39195678271308498</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="16"/>
+        <v>2.4009603841529947E-3</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
@@ -1725,6 +1872,13 @@
       <c r="B88" s="1">
         <v>0.37323511356660499</v>
       </c>
+      <c r="C88" s="1">
+        <v>0.35420503376304502</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.9030079803559974E-2</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
@@ -1733,6 +1887,13 @@
       <c r="B89" s="1">
         <v>0.44546568627451</v>
       </c>
+      <c r="C89" s="1">
+        <v>0.44852941176470601</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="16"/>
+        <v>3.063725490196012E-3</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
@@ -1741,135 +1902,151 @@
       <c r="B90" s="1">
         <v>0.53259237008110505</v>
       </c>
+      <c r="C90" s="1">
+        <v>0.49474316611595098</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="16"/>
+        <v>-3.7849203965154066E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="4"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B93" s="1">
-        <v>0.90138888888888902</v>
-      </c>
-      <c r="C93" s="1">
-        <v>0.86805555555555602</v>
-      </c>
-      <c r="D93" s="1">
-        <v>0.88472222222222197</v>
-      </c>
-      <c r="E93" s="1">
-        <v>0.88888888888888895</v>
-      </c>
-      <c r="F93" s="1">
-        <v>0.89861111111111103</v>
-      </c>
-      <c r="G93" s="1">
-        <v>0.86388888888888904</v>
+      <c r="D92" s="1">
+        <f>AVERAGE(D71:D90)</f>
+        <v>-1.4825864347648657E-2</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B95" s="1">
+        <v>0.90138888888888902</v>
+      </c>
+      <c r="C95" s="1">
+        <v>0.86805555555555602</v>
+      </c>
+      <c r="D95" s="1">
+        <v>0.88472222222222197</v>
+      </c>
+      <c r="E95" s="1">
+        <v>0.88888888888888895</v>
+      </c>
+      <c r="F95" s="1">
+        <v>0.89861111111111103</v>
+      </c>
+      <c r="G95" s="1">
+        <v>0.86388888888888904</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B96" s="1">
         <v>0.87083333333333302</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C96" s="1">
         <v>0.85972222222222205</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D96" s="1">
         <v>0.87083333333333302</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E96" s="1">
         <v>0.87083333333333302</v>
       </c>
-      <c r="F94" s="1">
+      <c r="F96" s="1">
         <v>0.87083333333333302</v>
       </c>
-      <c r="G94" s="1">
+      <c r="G96" s="1">
         <v>0.85416666666666696</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C96" s="1">
-        <f>C93-$B93</f>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C98" s="1">
+        <f>C95-$B95</f>
         <v>-3.3333333333332993E-2</v>
       </c>
-      <c r="D96" s="1">
-        <f>D93-$B93</f>
+      <c r="D98" s="1">
+        <f>D95-$B95</f>
         <v>-1.6666666666667052E-2</v>
       </c>
-      <c r="E96" s="1">
-        <f>E93-$B93</f>
+      <c r="E98" s="1">
+        <f>E95-$B95</f>
         <v>-1.2500000000000067E-2</v>
       </c>
-      <c r="F96" s="1">
-        <f>F93-$B93</f>
+      <c r="F98" s="1">
+        <f>F95-$B95</f>
         <v>-2.77777777777799E-3</v>
       </c>
-      <c r="G96" s="1">
-        <f>G93-$B93</f>
+      <c r="G98" s="1">
+        <f>G95-$B95</f>
         <v>-3.7499999999999978E-2</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C97" s="1">
-        <f>C94-B94</f>
-        <v>-1.1111111111110961E-2</v>
-      </c>
-      <c r="D97" s="1">
-        <f>D94-$B94</f>
-        <v>0</v>
-      </c>
-      <c r="E97" s="1">
-        <f>E94-$B94</f>
-        <v>0</v>
-      </c>
-      <c r="F97" s="1">
-        <f>F94-$B94</f>
-        <v>0</v>
-      </c>
-      <c r="G97" s="1">
-        <f>G94-$B94</f>
-        <v>-1.6666666666666052E-2</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B98" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C99" s="1">
-        <f>AVERAGE(C96:C97)</f>
+        <f>C96-B96</f>
+        <v>-1.1111111111110961E-2</v>
+      </c>
+      <c r="D99" s="1">
+        <f>D96-$B96</f>
+        <v>0</v>
+      </c>
+      <c r="E99" s="1">
+        <f>E96-$B96</f>
+        <v>0</v>
+      </c>
+      <c r="F99" s="1">
+        <f>F96-$B96</f>
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <f>G96-$B96</f>
+        <v>-1.6666666666666052E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B100" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C101" s="1">
+        <f>AVERAGE(C98:C99)</f>
         <v>-2.2222222222221977E-2</v>
       </c>
-      <c r="D99" s="1">
-        <f t="shared" ref="D99:G99" si="15">AVERAGE(D96:D97)</f>
+      <c r="D101" s="1">
+        <f t="shared" ref="D101:G101" si="17">AVERAGE(D98:D99)</f>
         <v>-8.3333333333335258E-3</v>
       </c>
-      <c r="E99" s="1">
-        <f t="shared" si="15"/>
+      <c r="E101" s="1">
+        <f t="shared" si="17"/>
         <v>-6.2500000000000333E-3</v>
       </c>
-      <c r="F99" s="1">
-        <f t="shared" si="15"/>
+      <c r="F101" s="1">
+        <f t="shared" si="17"/>
         <v>-1.388888888888995E-3</v>
       </c>
-      <c r="G99" s="1">
-        <f t="shared" si="15"/>
+      <c r="G101" s="1">
+        <f t="shared" si="17"/>
         <v>-2.7083333333333015E-2</v>
       </c>
     </row>

</xml_diff>